<commit_message>
Add supported prescription type for final example in supplier test-pack
</commit_message>
<xml_diff>
--- a/tool/e2e-tests/test-packs/Supplier 1 Test Pack.xlsx
+++ b/tool/e2e-tests/test-packs/Supplier 1 Test Pack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\clients\NHS\electronic-prescription-service-api\tool\e2e-tests\test-packs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621647CE-5F4D-40DF-89C0-081279B97E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA0A671-0481-473A-9F45-E710087E2C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{DE2866F1-D839-4AD2-B338-FF4A1D84F7C7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{DE2866F1-D839-4AD2-B338-FF4A1D84F7C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7079" uniqueCount="3352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7080" uniqueCount="3353">
   <si>
     <t>Quantity</t>
   </si>
@@ -10096,7 +10096,10 @@
     <t>0125</t>
   </si>
   <si>
-    <t>0200</t>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>Supported Prescription Types in Test-Packs so far: 0101, 0104, 0105, 0108, 0125 and 10**</t>
   </si>
 </sst>
 </file>
@@ -10234,10 +10237,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10537,10 +10536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7328C0-2D0B-4453-A6F9-9D47EA82D874}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10578,6 +10577,11 @@
         <v>3331</v>
       </c>
     </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>3352</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10588,9 +10592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90350D13-E130-47A5-A64D-77E01FA3003F}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Remove DIN number from practitioner in Supplier Test Pack and from fallback
</commit_message>
<xml_diff>
--- a/tool/e2e-tests/test-packs/Supplier 1 Test Pack.xlsx
+++ b/tool/e2e-tests/test-packs/Supplier 1 Test Pack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\clients\NHS\electronic-prescription-service-api\tool\e2e-tests\test-packs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDC016F-B5C4-437D-B426-F1AF6DBA0BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00425955-F602-49B1-97E4-10A524CB320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{DE2866F1-D839-4AD2-B338-FF4A1D84F7C7}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7518" uniqueCount="3423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7466" uniqueCount="3420">
   <si>
     <t>Quantity</t>
   </si>
@@ -10103,19 +10103,10 @@
     <t>Professional Code Type</t>
   </si>
   <si>
-    <t>Prescribing Code</t>
-  </si>
-  <si>
-    <t>Prescribing Code Type</t>
-  </si>
-  <si>
     <t>GMC</t>
   </si>
   <si>
     <t>C1234567</t>
-  </si>
-  <si>
-    <t>DIN</t>
   </si>
   <si>
     <t>Prescriber Name</t>
@@ -10807,7 +10798,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11128,7 +11119,7 @@
         <v>2</v>
       </c>
       <c r="R7" t="s">
-        <v>3422</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -11154,7 +11145,7 @@
         <v>28</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>3360</v>
+        <v>3357</v>
       </c>
       <c r="I8" s="2">
         <v>99999999</v>
@@ -11169,7 +11160,7 @@
         <v>11111111</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>3361</v>
+        <v>3358</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -11195,7 +11186,7 @@
         <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>3362</v>
+        <v>3359</v>
       </c>
       <c r="I9" s="2">
         <v>99999999</v>
@@ -11234,7 +11225,7 @@
         <v>28</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>3363</v>
+        <v>3360</v>
       </c>
       <c r="I10" s="2">
         <v>99999999</v>
@@ -11273,7 +11264,7 @@
         <v>28</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>3364</v>
+        <v>3361</v>
       </c>
       <c r="I11" s="2">
         <v>99999999</v>
@@ -11312,7 +11303,7 @@
         <v>28</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>3365</v>
+        <v>3362</v>
       </c>
       <c r="I12" s="2">
         <v>99999999</v>
@@ -11351,7 +11342,7 @@
         <v>28</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>3366</v>
+        <v>3363</v>
       </c>
       <c r="I13" s="2">
         <v>99999999</v>
@@ -11360,13 +11351,13 @@
         <v>15</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>3367</v>
+        <v>3364</v>
       </c>
       <c r="L13" s="2">
         <v>11111111</v>
       </c>
       <c r="M13" s="18" t="s">
-        <v>3368</v>
+        <v>3365</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -11392,7 +11383,7 @@
         <v>28</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>3369</v>
+        <v>3366</v>
       </c>
       <c r="I14" s="2">
         <v>99999999</v>
@@ -11431,7 +11422,7 @@
         <v>28</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>3370</v>
+        <v>3367</v>
       </c>
       <c r="I15" s="2">
         <v>99999999</v>
@@ -11440,7 +11431,7 @@
         <v>60</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>3371</v>
+        <v>3368</v>
       </c>
       <c r="L15" s="2">
         <v>11111111</v>
@@ -11470,7 +11461,7 @@
         <v>28</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>3372</v>
+        <v>3369</v>
       </c>
       <c r="I16" s="2">
         <v>99999999</v>
@@ -11509,7 +11500,7 @@
         <v>28</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>3373</v>
+        <v>3370</v>
       </c>
       <c r="I17" s="2">
         <v>99999999</v>
@@ -11518,7 +11509,7 @@
         <v>56</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>3367</v>
+        <v>3364</v>
       </c>
       <c r="L17" s="2">
         <v>11111111</v>
@@ -11548,7 +11539,7 @@
         <v>28</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>3374</v>
+        <v>3371</v>
       </c>
       <c r="I18" s="2">
         <v>99999999</v>
@@ -11557,7 +11548,7 @@
         <v>50</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>3375</v>
+        <v>3372</v>
       </c>
       <c r="L18" s="2">
         <v>11111111</v>
@@ -11587,7 +11578,7 @@
         <v>28</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>3376</v>
+        <v>3373</v>
       </c>
       <c r="I19" s="2">
         <v>99999999</v>
@@ -11596,7 +11587,7 @@
         <v>68</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>3371</v>
+        <v>3368</v>
       </c>
       <c r="L19" s="2">
         <v>11111111</v>
@@ -11626,7 +11617,7 @@
         <v>28</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>3377</v>
+        <v>3374</v>
       </c>
       <c r="I20" s="2">
         <v>99999999</v>
@@ -11635,7 +11626,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>3378</v>
+        <v>3375</v>
       </c>
       <c r="L20" s="2">
         <v>11111111</v>
@@ -11665,7 +11656,7 @@
         <v>28</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>3379</v>
+        <v>3376</v>
       </c>
       <c r="I21" s="2">
         <v>99999999</v>
@@ -11704,7 +11695,7 @@
         <v>28</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>3380</v>
+        <v>3377</v>
       </c>
       <c r="I22" s="2">
         <v>99999999</v>
@@ -11713,7 +11704,7 @@
         <v>20</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>3381</v>
+        <v>3378</v>
       </c>
       <c r="L22" s="2">
         <v>11111111</v>
@@ -11743,7 +11734,7 @@
         <v>28</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>3382</v>
+        <v>3379</v>
       </c>
       <c r="I23" s="2">
         <v>99999999</v>
@@ -11782,7 +11773,7 @@
         <v>28</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>3383</v>
+        <v>3380</v>
       </c>
       <c r="I24" s="2">
         <v>99999999</v>
@@ -11791,7 +11782,7 @@
         <v>20</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>3384</v>
+        <v>3381</v>
       </c>
       <c r="L24" s="2">
         <v>11111111</v>
@@ -11821,7 +11812,7 @@
         <v>28</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>3385</v>
+        <v>3382</v>
       </c>
       <c r="I25" s="2">
         <v>99999999</v>
@@ -11860,7 +11851,7 @@
         <v>28</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>3386</v>
+        <v>3383</v>
       </c>
       <c r="I26" s="2">
         <v>99999999</v>
@@ -11899,7 +11890,7 @@
         <v>28</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>3387</v>
+        <v>3384</v>
       </c>
       <c r="I27" s="2">
         <v>99999999</v>
@@ -11908,7 +11899,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>3388</v>
+        <v>3385</v>
       </c>
       <c r="L27" s="2">
         <v>11111111</v>
@@ -11938,7 +11929,7 @@
         <v>28</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>3389</v>
+        <v>3386</v>
       </c>
       <c r="I28" s="2">
         <v>99999999</v>
@@ -11977,7 +11968,7 @@
         <v>28</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>3390</v>
+        <v>3387</v>
       </c>
       <c r="I29" s="2">
         <v>99999999</v>
@@ -12016,7 +12007,7 @@
         <v>28</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>3391</v>
+        <v>3388</v>
       </c>
       <c r="I30" s="2">
         <v>99999999</v>
@@ -12055,7 +12046,7 @@
         <v>28</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>3392</v>
+        <v>3389</v>
       </c>
       <c r="I31" s="2">
         <v>99999999</v>
@@ -12064,7 +12055,7 @@
         <v>3</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>3367</v>
+        <v>3364</v>
       </c>
       <c r="L31" s="2">
         <v>11111111</v>
@@ -12094,7 +12085,7 @@
         <v>28</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>3393</v>
+        <v>3390</v>
       </c>
       <c r="I32" s="2">
         <v>99999999</v>
@@ -12133,7 +12124,7 @@
         <v>28</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>3394</v>
+        <v>3391</v>
       </c>
       <c r="I33" s="2">
         <v>99999999</v>
@@ -12142,7 +12133,7 @@
         <v>14</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>3395</v>
+        <v>3392</v>
       </c>
       <c r="L33" s="2">
         <v>11111111</v>
@@ -12175,7 +12166,7 @@
         <v>28</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>3396</v>
+        <v>3393</v>
       </c>
       <c r="I34" s="2">
         <v>99999999</v>
@@ -12184,7 +12175,7 @@
         <v>200</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>3371</v>
+        <v>3368</v>
       </c>
       <c r="L34" s="2">
         <v>11111111</v>
@@ -12214,7 +12205,7 @@
         <v>28</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>3397</v>
+        <v>3394</v>
       </c>
       <c r="I35" s="2">
         <v>99999999</v>
@@ -12230,7 +12221,7 @@
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="17" t="s">
-        <v>3398</v>
+        <v>3395</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -12256,7 +12247,7 @@
         <v>28</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>3399</v>
+        <v>3396</v>
       </c>
       <c r="I36" s="2">
         <v>99999999</v>
@@ -12272,7 +12263,7 @@
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="17" t="s">
-        <v>3400</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -12298,7 +12289,7 @@
         <v>28</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>3401</v>
+        <v>3398</v>
       </c>
       <c r="I37" s="2">
         <v>99999999</v>
@@ -12307,7 +12298,7 @@
         <v>24</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>3395</v>
+        <v>3392</v>
       </c>
       <c r="L37" s="2">
         <v>11111111</v>
@@ -12336,7 +12327,7 @@
         <v>28</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>3402</v>
+        <v>3399</v>
       </c>
       <c r="I38" s="2">
         <v>99999999</v>
@@ -12375,7 +12366,7 @@
         <v>28</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>3403</v>
+        <v>3400</v>
       </c>
       <c r="I39" s="2">
         <v>99999999</v>
@@ -12414,7 +12405,7 @@
         <v>28</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>3404</v>
+        <v>3401</v>
       </c>
       <c r="I40" s="2">
         <v>99999999</v>
@@ -12423,7 +12414,7 @@
         <v>6</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>3395</v>
+        <v>3392</v>
       </c>
       <c r="L40" s="2">
         <v>11111111</v>
@@ -12453,7 +12444,7 @@
         <v>28</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>3405</v>
+        <v>3402</v>
       </c>
       <c r="I41" s="2">
         <v>99999999</v>
@@ -12462,7 +12453,7 @@
         <v>30</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>3406</v>
+        <v>3403</v>
       </c>
       <c r="L41" s="2">
         <v>11111111</v>
@@ -12492,7 +12483,7 @@
         <v>28</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>3407</v>
+        <v>3404</v>
       </c>
       <c r="I42" s="2">
         <v>99999999</v>
@@ -12532,7 +12523,7 @@
         <v>28</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>3408</v>
+        <v>3405</v>
       </c>
       <c r="I43" s="2">
         <v>99999999</v>
@@ -12571,7 +12562,7 @@
         <v>28</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>3409</v>
+        <v>3406</v>
       </c>
       <c r="I44" s="2">
         <v>99999999</v>
@@ -12580,7 +12571,7 @@
         <v>5</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>3410</v>
+        <v>3407</v>
       </c>
       <c r="L44" s="2">
         <v>11111111</v>
@@ -12610,7 +12601,7 @@
         <v>28</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>3411</v>
+        <v>3408</v>
       </c>
       <c r="I45" s="2">
         <v>99999999</v>
@@ -12619,7 +12610,7 @@
         <v>2</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>3412</v>
+        <v>3409</v>
       </c>
       <c r="L45" s="2">
         <v>11111111</v>
@@ -12649,7 +12640,7 @@
         <v>28</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>3413</v>
+        <v>3410</v>
       </c>
       <c r="I46" s="2">
         <v>99999999</v>
@@ -12664,7 +12655,7 @@
         <v>11111111</v>
       </c>
       <c r="M46" s="18" t="s">
-        <v>3414</v>
+        <v>3411</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -12690,7 +12681,7 @@
         <v>28</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>3415</v>
+        <v>3412</v>
       </c>
       <c r="I47" s="2">
         <v>99999999</v>
@@ -12699,7 +12690,7 @@
         <v>14</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>3367</v>
+        <v>3364</v>
       </c>
       <c r="L47" s="2">
         <v>11111111</v>
@@ -12729,7 +12720,7 @@
         <v>28</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>3416</v>
+        <v>3413</v>
       </c>
       <c r="I48" s="2">
         <v>99999999</v>
@@ -12768,7 +12759,7 @@
         <v>28</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>3417</v>
+        <v>3414</v>
       </c>
       <c r="I49" s="2">
         <v>99999999</v>
@@ -12777,7 +12768,7 @@
         <v>2</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>3418</v>
+        <v>3415</v>
       </c>
       <c r="L49" s="2">
         <v>11111111</v>
@@ -12807,7 +12798,7 @@
         <v>28</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>3419</v>
+        <v>3416</v>
       </c>
       <c r="I50" s="2">
         <v>99999999</v>
@@ -12816,14 +12807,14 @@
         <v>30</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>3395</v>
+        <v>3392</v>
       </c>
       <c r="L50" s="2">
         <v>11111111</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" s="17" t="s">
-        <v>3420</v>
+        <v>3417</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -12849,7 +12840,7 @@
         <v>28</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>3421</v>
+        <v>3418</v>
       </c>
       <c r="I51" s="2">
         <v>99999999</v>
@@ -47023,27 +47014,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4197C79A-0579-4860-90D6-E5D60D4D545C}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.04296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.2265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3358</v>
+        <v>3355</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>3351</v>
@@ -47051,1011 +47038,705 @@
       <c r="D1" s="7" t="s">
         <v>3352</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>3353</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>3354</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D2" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E2">
-        <v>70201123456</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D3" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E3">
-        <v>70201123456</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D4" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E4">
-        <v>70201123456</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D5" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E5">
-        <v>70201123456</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D6" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E6">
-        <v>70201123456</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D7" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E7">
-        <v>70201123456</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D8" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E8">
-        <v>70201123456</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D9" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E9">
-        <v>70201123456</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D10" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E10">
-        <v>70201123456</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D11" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E11">
-        <v>70201123456</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D12" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E12">
-        <v>70201123456</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D13" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E13">
-        <v>70201123456</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D14" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E14">
-        <v>70201123456</v>
-      </c>
-      <c r="F14" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D15" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E15">
-        <v>70201123456</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D16" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E16">
-        <v>70201123456</v>
-      </c>
-      <c r="F16" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D17" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E17">
-        <v>70201123456</v>
-      </c>
-      <c r="F17" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D18" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E18">
-        <v>70201123456</v>
-      </c>
-      <c r="F18" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D19" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E19">
-        <v>70201123456</v>
-      </c>
-      <c r="F19" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D20" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E20">
-        <v>70201123456</v>
-      </c>
-      <c r="F20" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D21" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E21">
-        <v>70201123456</v>
-      </c>
-      <c r="F21" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D22" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E22">
-        <v>70201123456</v>
-      </c>
-      <c r="F22" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D23" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E23">
-        <v>70201123456</v>
-      </c>
-      <c r="F23" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D24" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E24">
-        <v>70201123456</v>
-      </c>
-      <c r="F24" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D25" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E25">
-        <v>70201123456</v>
-      </c>
-      <c r="F25" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D26" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E26">
-        <v>70201123456</v>
-      </c>
-      <c r="F26" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D27" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E27">
-        <v>70201123456</v>
-      </c>
-      <c r="F27" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D28" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E28">
-        <v>70201123456</v>
-      </c>
-      <c r="F28" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D29" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E29">
-        <v>70201123456</v>
-      </c>
-      <c r="F29" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D30" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E30">
-        <v>70201123456</v>
-      </c>
-      <c r="F30" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D31" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E31">
-        <v>70201123456</v>
-      </c>
-      <c r="F31" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D32" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E32">
-        <v>70201123456</v>
-      </c>
-      <c r="F32" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D33" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E33">
-        <v>70201123456</v>
-      </c>
-      <c r="F33" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D34" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E34">
-        <v>70201123456</v>
-      </c>
-      <c r="F34" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D35" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E35">
-        <v>70201123456</v>
-      </c>
-      <c r="F35" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D36" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E36">
-        <v>70201123456</v>
-      </c>
-      <c r="F36" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D37" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E37">
-        <v>70201123456</v>
-      </c>
-      <c r="F37" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D38" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E38">
-        <v>70201123456</v>
-      </c>
-      <c r="F38" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D39" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E39">
-        <v>70201123456</v>
-      </c>
-      <c r="F39" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D40" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E40">
-        <v>70201123456</v>
-      </c>
-      <c r="F40" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D41" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E41">
-        <v>70201123456</v>
-      </c>
-      <c r="F41" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D42" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E42">
-        <v>70201123456</v>
-      </c>
-      <c r="F42" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D43" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E43">
-        <v>70201123456</v>
-      </c>
-      <c r="F43" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D44" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E44">
-        <v>70201123456</v>
-      </c>
-      <c r="F44" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D45" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E45">
-        <v>70201123456</v>
-      </c>
-      <c r="F45" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D46" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E46">
-        <v>70201123456</v>
-      </c>
-      <c r="F46" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D47" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E47">
-        <v>70201123456</v>
-      </c>
-      <c r="F47" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D48" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E48">
-        <v>70201123456</v>
-      </c>
-      <c r="F48" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
       <c r="C49" s="14" t="s">
+        <v>3354</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>3356</v>
       </c>
-      <c r="D49" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E49">
-        <v>70201123456</v>
-      </c>
-      <c r="F49" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>3359</v>
-      </c>
       <c r="C50" s="14" t="s">
+        <v>3354</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>3356</v>
       </c>
-      <c r="D50" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E50">
-        <v>70201123456</v>
-      </c>
-      <c r="F50" t="s">
-        <v>3357</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>3359</v>
-      </c>
       <c r="C51" s="14" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="D51" t="s">
-        <v>3355</v>
-      </c>
-      <c r="E51">
-        <v>70201123456</v>
-      </c>
-      <c r="F51" t="s">
-        <v>3357</v>
+        <v>3353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>